<commit_message>
Update packages through to 5th April 2026 year ends.
</commit_message>
<xml_diff>
--- a/GB Accounts 2025-26/GB Accounts Company 2025-2026 (Any) Excel 2007/Fixedassets.xlsx
+++ b/GB Accounts 2025-26/GB Accounts Company 2025-2026 (Any) Excel 2007/Fixedassets.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10329"/>
   <workbookPr showObjects="placeholders" codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antony/projects/diy-accounting/GB Accounts 2024-25/GB Accounts Company 2024-2025 (Any) Excel 2007/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/antony/projects/diy-accounting/GB Accounts 2025-26/GB Accounts Company 2025-2026 (Any) Excel 2007/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B39AF71-5574-C246-8F9D-B12326CCF553}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA0EC991-CEDD-3944-A060-92AFF66B1EB6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="24560" windowHeight="16980" tabRatio="724" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1040,31 +1040,55 @@
     <xf numFmtId="1" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="15" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="164" fontId="2" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -1090,8 +1114,11 @@
     <xf numFmtId="164" fontId="4" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="165" fontId="3" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1105,54 +1132,65 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="15" fontId="2" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="6"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="6"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1" indent="6"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" indent="6"/>
     </xf>
@@ -1174,43 +1212,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1" indent="6"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="4" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="3" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="4" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
@@ -1218,20 +1227,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="2"/>
     </xf>
-    <xf numFmtId="4" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="1" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1290,7 +1290,7 @@
         </row>
         <row r="6">
           <cell r="L6">
-            <v>45413</v>
+            <v>45778</v>
           </cell>
         </row>
         <row r="7">
@@ -1298,7 +1298,7 @@
             <v>100</v>
           </cell>
           <cell r="N7">
-            <v>46142</v>
+            <v>46507</v>
           </cell>
         </row>
         <row r="11">
@@ -1309,7 +1309,7 @@
             <v>3000</v>
           </cell>
           <cell r="N11">
-            <v>45777</v>
+            <v>46142</v>
           </cell>
         </row>
       </sheetData>
@@ -1644,14 +1644,14 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:27" s="6" customFormat="1" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="133"/>
-      <c r="B1" s="138" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="135" t="s">
+      <c r="A1" s="141"/>
+      <c r="B1" s="122" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="143" t="s">
         <v>7</v>
       </c>
-      <c r="D1" s="136"/>
+      <c r="D1" s="144"/>
       <c r="E1" s="61">
         <f>E57+E110</f>
         <v>0</v>
@@ -1664,7 +1664,7 @@
         <f>G57+G110</f>
         <v>0</v>
       </c>
-      <c r="H1" s="122" t="s">
+      <c r="H1" s="152" t="s">
         <v>10</v>
       </c>
       <c r="I1" s="19">
@@ -1679,16 +1679,16 @@
         <f>K57+K110</f>
         <v>0</v>
       </c>
-      <c r="L1" s="149"/>
-      <c r="M1" s="122" t="s">
+      <c r="L1" s="128"/>
+      <c r="M1" s="152" t="s">
         <v>5</v>
       </c>
-      <c r="N1" s="149"/>
+      <c r="N1" s="128"/>
       <c r="O1" s="19">
         <f>O57+O110</f>
         <v>0</v>
       </c>
-      <c r="P1" s="154" t="s">
+      <c r="P1" s="133" t="s">
         <v>63</v>
       </c>
       <c r="Q1" s="19">
@@ -1703,8 +1703,8 @@
         <f>S57+S110</f>
         <v>0</v>
       </c>
-      <c r="T1" s="149"/>
-      <c r="U1" s="145" t="s">
+      <c r="T1" s="128"/>
+      <c r="U1" s="121" t="s">
         <v>31</v>
       </c>
       <c r="V1" s="19">
@@ -1730,146 +1730,146 @@
       <c r="AA1" s="20"/>
     </row>
     <row r="2" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A2" s="134"/>
-      <c r="B2" s="138"/>
-      <c r="C2" s="146" t="s">
+      <c r="A2" s="142"/>
+      <c r="B2" s="122"/>
+      <c r="C2" s="123" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="148" t="s">
+      <c r="D2" s="125" t="s">
         <v>2</v>
       </c>
-      <c r="E2" s="144" t="s">
+      <c r="E2" s="120" t="s">
         <v>3</v>
       </c>
-      <c r="F2" s="125" t="s">
+      <c r="F2" s="155" t="s">
         <v>56</v>
       </c>
-      <c r="G2" s="127" t="s">
+      <c r="G2" s="126" t="s">
         <v>62</v>
       </c>
-      <c r="H2" s="124"/>
-      <c r="I2" s="137" t="s">
+      <c r="H2" s="154"/>
+      <c r="I2" s="145" t="s">
         <v>16</v>
       </c>
-      <c r="J2" s="125" t="s">
+      <c r="J2" s="155" t="s">
         <v>56</v>
       </c>
-      <c r="K2" s="127" t="s">
+      <c r="K2" s="126" t="s">
         <v>62</v>
       </c>
-      <c r="L2" s="150"/>
-      <c r="M2" s="123"/>
-      <c r="N2" s="150"/>
-      <c r="O2" s="127" t="s">
+      <c r="L2" s="129"/>
+      <c r="M2" s="153"/>
+      <c r="N2" s="129"/>
+      <c r="O2" s="126" t="s">
         <v>61</v>
       </c>
-      <c r="P2" s="155"/>
-      <c r="Q2" s="127" t="s">
+      <c r="P2" s="134"/>
+      <c r="Q2" s="126" t="s">
         <v>64</v>
       </c>
-      <c r="R2" s="127" t="s">
+      <c r="R2" s="126" t="s">
         <v>4</v>
       </c>
-      <c r="S2" s="127" t="s">
+      <c r="S2" s="126" t="s">
         <v>61</v>
       </c>
-      <c r="T2" s="156"/>
-      <c r="U2" s="138"/>
-      <c r="V2" s="143" t="s">
+      <c r="T2" s="135"/>
+      <c r="U2" s="122"/>
+      <c r="V2" s="136" t="s">
         <v>29</v>
       </c>
-      <c r="W2" s="143" t="s">
+      <c r="W2" s="136" t="s">
         <v>30</v>
       </c>
-      <c r="X2" s="143" t="s">
+      <c r="X2" s="136" t="s">
         <v>32</v>
       </c>
-      <c r="Y2" s="144" t="s">
+      <c r="Y2" s="120" t="s">
         <v>49</v>
       </c>
-      <c r="Z2" s="144" t="s">
+      <c r="Z2" s="120" t="s">
         <v>50</v>
       </c>
       <c r="AA2" s="21"/>
     </row>
     <row r="3" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="134"/>
-      <c r="B3" s="138"/>
-      <c r="C3" s="147"/>
-      <c r="D3" s="148"/>
-      <c r="E3" s="144"/>
-      <c r="F3" s="126"/>
-      <c r="G3" s="128"/>
-      <c r="H3" s="124"/>
-      <c r="I3" s="137"/>
-      <c r="J3" s="126"/>
-      <c r="K3" s="128"/>
-      <c r="L3" s="150"/>
-      <c r="M3" s="123"/>
-      <c r="N3" s="150"/>
-      <c r="O3" s="128"/>
-      <c r="P3" s="155"/>
-      <c r="Q3" s="152"/>
-      <c r="R3" s="128"/>
-      <c r="S3" s="128"/>
-      <c r="T3" s="156"/>
-      <c r="U3" s="138"/>
-      <c r="V3" s="144"/>
-      <c r="W3" s="144"/>
-      <c r="X3" s="144"/>
-      <c r="Y3" s="144"/>
-      <c r="Z3" s="144"/>
+      <c r="A3" s="142"/>
+      <c r="B3" s="122"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="125"/>
+      <c r="E3" s="120"/>
+      <c r="F3" s="156"/>
+      <c r="G3" s="127"/>
+      <c r="H3" s="154"/>
+      <c r="I3" s="145"/>
+      <c r="J3" s="156"/>
+      <c r="K3" s="127"/>
+      <c r="L3" s="129"/>
+      <c r="M3" s="153"/>
+      <c r="N3" s="129"/>
+      <c r="O3" s="127"/>
+      <c r="P3" s="134"/>
+      <c r="Q3" s="131"/>
+      <c r="R3" s="127"/>
+      <c r="S3" s="127"/>
+      <c r="T3" s="135"/>
+      <c r="U3" s="122"/>
+      <c r="V3" s="120"/>
+      <c r="W3" s="120"/>
+      <c r="X3" s="120"/>
+      <c r="Y3" s="120"/>
+      <c r="Z3" s="120"/>
       <c r="AA3" s="21"/>
     </row>
     <row r="4" spans="1:27" s="15" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="134"/>
-      <c r="B4" s="138"/>
-      <c r="C4" s="147"/>
-      <c r="D4" s="148"/>
-      <c r="E4" s="144"/>
+      <c r="A4" s="142"/>
+      <c r="B4" s="122"/>
+      <c r="C4" s="124"/>
+      <c r="D4" s="125"/>
+      <c r="E4" s="120"/>
       <c r="F4" s="111">
         <f>D6</f>
-        <v>45413</v>
+        <v>45778</v>
       </c>
       <c r="G4" s="111">
         <f>D6</f>
-        <v>45413</v>
-      </c>
-      <c r="H4" s="124"/>
-      <c r="I4" s="137"/>
+        <v>45778</v>
+      </c>
+      <c r="H4" s="154"/>
+      <c r="I4" s="145"/>
       <c r="J4" s="111">
         <f>[1]Admin!$N$7</f>
-        <v>46142</v>
+        <v>46507</v>
       </c>
       <c r="K4" s="111">
         <f>J4</f>
-        <v>46142</v>
-      </c>
-      <c r="L4" s="151"/>
-      <c r="M4" s="123"/>
-      <c r="N4" s="151"/>
+        <v>46507</v>
+      </c>
+      <c r="L4" s="130"/>
+      <c r="M4" s="153"/>
+      <c r="N4" s="130"/>
       <c r="O4" s="110">
         <f>D6</f>
-        <v>45413</v>
+        <v>45778</v>
       </c>
       <c r="P4" s="119">
         <v>100</v>
       </c>
-      <c r="Q4" s="153"/>
+      <c r="Q4" s="132"/>
       <c r="R4" s="118">
         <v>20</v>
       </c>
       <c r="S4" s="110">
         <f>J4</f>
-        <v>46142</v>
-      </c>
-      <c r="T4" s="156"/>
-      <c r="U4" s="138"/>
-      <c r="V4" s="144"/>
-      <c r="W4" s="144"/>
-      <c r="X4" s="144"/>
-      <c r="Y4" s="144"/>
-      <c r="Z4" s="144"/>
+        <v>46507</v>
+      </c>
+      <c r="T4" s="135"/>
+      <c r="U4" s="122"/>
+      <c r="V4" s="120"/>
+      <c r="W4" s="120"/>
+      <c r="X4" s="120"/>
+      <c r="Y4" s="120"/>
+      <c r="Z4" s="120"/>
       <c r="AA4" s="22"/>
     </row>
     <row r="5" spans="1:27" s="15" customFormat="1" ht="6" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
@@ -1903,15 +1903,15 @@
     </row>
     <row r="6" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A6" s="100"/>
-      <c r="B6" s="120" t="s">
+      <c r="B6" s="146" t="s">
         <v>57</v>
       </c>
-      <c r="C6" s="121"/>
-      <c r="D6" s="139">
+      <c r="C6" s="147"/>
+      <c r="D6" s="148">
         <f>[1]Admin!$L$6</f>
-        <v>45413</v>
-      </c>
-      <c r="E6" s="140"/>
+        <v>45778</v>
+      </c>
+      <c r="E6" s="149"/>
       <c r="F6" s="8"/>
       <c r="G6" s="8"/>
       <c r="H6" s="9"/>
@@ -1937,10 +1937,10 @@
     </row>
     <row r="7" spans="1:27" ht="13.5" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="100"/>
-      <c r="B7" s="129" t="s">
+      <c r="B7" s="137" t="s">
         <v>9</v>
       </c>
-      <c r="C7" s="129"/>
+      <c r="C7" s="137"/>
       <c r="D7" s="29"/>
       <c r="E7" s="8"/>
       <c r="F7" s="8"/>
@@ -2120,12 +2120,12 @@
     </row>
     <row r="11" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A11" s="100"/>
-      <c r="B11" s="130" t="str">
+      <c r="B11" s="138" t="str">
         <f>IF((E11-F11)=([1]OpenAccounts!$G$13-[1]OpenAccounts!$M$13),"Existing Land &amp; Property","Check Opening Balance Sheet figures agree")</f>
         <v>Existing Land &amp; Property</v>
       </c>
-      <c r="C11" s="131"/>
-      <c r="D11" s="132"/>
+      <c r="C11" s="139"/>
+      <c r="D11" s="140"/>
       <c r="E11" s="40">
         <f>SUM(E8:E10)</f>
         <v>0</v>
@@ -2226,10 +2226,10 @@
     </row>
     <row r="13" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A13" s="100"/>
-      <c r="B13" s="129" t="s">
+      <c r="B13" s="137" t="s">
         <v>8</v>
       </c>
-      <c r="C13" s="129"/>
+      <c r="C13" s="137"/>
       <c r="D13" s="31"/>
       <c r="E13" s="7"/>
       <c r="F13" s="7"/>
@@ -2755,12 +2755,12 @@
     </row>
     <row r="22" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A22" s="100"/>
-      <c r="B22" s="130" t="str">
+      <c r="B22" s="138" t="str">
         <f>IF((E22-F22)=([1]OpenAccounts!$H$13-[1]OpenAccounts!$N$13),"Existing Plant &amp; Machinery", "Check Opening Balance Sheet figures agree")</f>
         <v>Existing Plant &amp; Machinery</v>
       </c>
-      <c r="C22" s="131"/>
-      <c r="D22" s="132"/>
+      <c r="C22" s="139"/>
+      <c r="D22" s="140"/>
       <c r="E22" s="40">
         <f>SUM(E14:E21)</f>
         <v>0</v>
@@ -2861,10 +2861,10 @@
     </row>
     <row r="24" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A24" s="100"/>
-      <c r="B24" s="129" t="s">
+      <c r="B24" s="137" t="s">
         <v>55</v>
       </c>
-      <c r="C24" s="129"/>
+      <c r="C24" s="137"/>
       <c r="D24" s="31"/>
       <c r="E24" s="7"/>
       <c r="F24" s="7"/>
@@ -3204,12 +3204,12 @@
     </row>
     <row r="30" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A30" s="100"/>
-      <c r="B30" s="130" t="str">
+      <c r="B30" s="138" t="str">
         <f>IF((E30-F30)=([1]OpenAccounts!$I$13-[1]OpenAccounts!$O$13),"Existing Fixtures &amp; Fittings","Check Opening Balance Sheet figures agree")</f>
         <v>Existing Fixtures &amp; Fittings</v>
       </c>
-      <c r="C30" s="131"/>
-      <c r="D30" s="132"/>
+      <c r="C30" s="139"/>
+      <c r="D30" s="140"/>
       <c r="E30" s="40">
         <f>SUM(E25:E29)</f>
         <v>0</v>
@@ -3310,10 +3310,10 @@
     </row>
     <row r="32" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A32" s="100"/>
-      <c r="B32" s="129" t="s">
+      <c r="B32" s="137" t="s">
         <v>6</v>
       </c>
-      <c r="C32" s="129"/>
+      <c r="C32" s="137"/>
       <c r="D32" s="32"/>
       <c r="E32" s="7"/>
       <c r="F32" s="7"/>
@@ -3839,12 +3839,12 @@
     </row>
     <row r="41" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A41" s="100"/>
-      <c r="B41" s="130" t="str">
+      <c r="B41" s="138" t="str">
         <f>IF((E41-F41)=([1]OpenAccounts!$J$13-[1]OpenAccounts!$P$13),"Existing Computers","Check Opening Balkance Sheet figures agree")</f>
         <v>Existing Computers</v>
       </c>
-      <c r="C41" s="131"/>
-      <c r="D41" s="132"/>
+      <c r="C41" s="139"/>
+      <c r="D41" s="140"/>
       <c r="E41" s="40">
         <f>SUM(E33:E40)</f>
         <v>0</v>
@@ -3945,10 +3945,10 @@
     </row>
     <row r="43" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A43" s="100"/>
-      <c r="B43" s="129" t="s">
+      <c r="B43" s="137" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="129"/>
+      <c r="C43" s="137"/>
       <c r="D43" s="32"/>
       <c r="E43" s="7"/>
       <c r="F43" s="7"/>
@@ -4298,10 +4298,10 @@
     </row>
     <row r="49" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A49" s="100"/>
-      <c r="B49" s="129" t="s">
+      <c r="B49" s="137" t="s">
         <v>54</v>
       </c>
-      <c r="C49" s="129"/>
+      <c r="C49" s="137"/>
       <c r="D49" s="31"/>
       <c r="E49" s="7"/>
       <c r="F49" s="7"/>
@@ -4649,12 +4649,12 @@
     </row>
     <row r="55" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A55" s="100"/>
-      <c r="B55" s="130" t="str">
+      <c r="B55" s="138" t="str">
         <f>IF((E55-F55)=([1]OpenAccounts!$K$13-[1]OpenAccounts!$Q$13),"Existing Motor Vehicles","Check Opening Balance Sheet figures agree")</f>
         <v>Existing Motor Vehicles</v>
       </c>
-      <c r="C55" s="131"/>
-      <c r="D55" s="132"/>
+      <c r="C55" s="139"/>
+      <c r="D55" s="140"/>
       <c r="E55" s="40">
         <f>SUM(E44:E54)</f>
         <v>0</v>
@@ -4755,14 +4755,14 @@
     </row>
     <row r="57" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A57" s="100"/>
-      <c r="B57" s="120" t="str">
+      <c r="B57" s="146" t="str">
         <f>B6</f>
         <v xml:space="preserve">EXISTING FIXED ASSETS AT </v>
       </c>
-      <c r="C57" s="121"/>
+      <c r="C57" s="147"/>
       <c r="D57" s="115">
         <f>D6</f>
-        <v>45413</v>
+        <v>45778</v>
       </c>
       <c r="E57" s="18">
         <f>E11+E22+E30+E41+E55</f>
@@ -4864,20 +4864,20 @@
     </row>
     <row r="59" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A59" s="100"/>
-      <c r="B59" s="141" t="s">
+      <c r="B59" s="150" t="s">
         <v>58</v>
       </c>
-      <c r="C59" s="142"/>
+      <c r="C59" s="151"/>
       <c r="D59" s="116">
         <f>D57</f>
-        <v>45413</v>
+        <v>45778</v>
       </c>
       <c r="E59" s="113" t="s">
         <v>59</v>
       </c>
       <c r="F59" s="117">
         <f>J4</f>
-        <v>46142</v>
+        <v>46507</v>
       </c>
       <c r="G59" s="114"/>
       <c r="H59" s="13"/>
@@ -4903,10 +4903,10 @@
     </row>
     <row r="60" spans="1:27" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A60" s="100"/>
-      <c r="B60" s="129" t="s">
+      <c r="B60" s="137" t="s">
         <v>9</v>
       </c>
-      <c r="C60" s="129"/>
+      <c r="C60" s="137"/>
       <c r="D60" s="29"/>
       <c r="E60" s="8"/>
       <c r="F60" s="114"/>
@@ -5078,11 +5078,11 @@
     </row>
     <row r="64" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A64" s="100"/>
-      <c r="B64" s="130" t="s">
+      <c r="B64" s="138" t="s">
         <v>11</v>
       </c>
-      <c r="C64" s="131"/>
-      <c r="D64" s="132"/>
+      <c r="C64" s="139"/>
+      <c r="D64" s="140"/>
       <c r="E64" s="40">
         <f>SUM(E61:E63)</f>
         <v>0</v>
@@ -5183,10 +5183,10 @@
     </row>
     <row r="66" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A66" s="100"/>
-      <c r="B66" s="129" t="s">
+      <c r="B66" s="137" t="s">
         <v>8</v>
       </c>
-      <c r="C66" s="129"/>
+      <c r="C66" s="137"/>
       <c r="D66" s="31"/>
       <c r="E66" s="7"/>
       <c r="F66" s="7"/>
@@ -5713,11 +5713,11 @@
     </row>
     <row r="75" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A75" s="100"/>
-      <c r="B75" s="130" t="s">
+      <c r="B75" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="C75" s="131"/>
-      <c r="D75" s="132"/>
+      <c r="C75" s="139"/>
+      <c r="D75" s="140"/>
       <c r="E75" s="40">
         <f>SUM(E67:E74)</f>
         <v>0</v>
@@ -5818,10 +5818,10 @@
     </row>
     <row r="77" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A77" s="100"/>
-      <c r="B77" s="129" t="s">
+      <c r="B77" s="137" t="s">
         <v>55</v>
       </c>
-      <c r="C77" s="129"/>
+      <c r="C77" s="137"/>
       <c r="D77" s="31"/>
       <c r="E77" s="7"/>
       <c r="F77" s="7"/>
@@ -6162,11 +6162,11 @@
     </row>
     <row r="83" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A83" s="100"/>
-      <c r="B83" s="130" t="s">
+      <c r="B83" s="138" t="s">
         <v>13</v>
       </c>
-      <c r="C83" s="131"/>
-      <c r="D83" s="132"/>
+      <c r="C83" s="139"/>
+      <c r="D83" s="140"/>
       <c r="E83" s="40">
         <f>SUM(E78:E82)</f>
         <v>0</v>
@@ -6267,10 +6267,10 @@
     </row>
     <row r="85" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A85" s="100"/>
-      <c r="B85" s="129" t="s">
+      <c r="B85" s="137" t="s">
         <v>6</v>
       </c>
-      <c r="C85" s="129"/>
+      <c r="C85" s="137"/>
       <c r="D85" s="32"/>
       <c r="E85" s="7"/>
       <c r="F85" s="7"/>
@@ -6797,11 +6797,11 @@
     </row>
     <row r="94" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A94" s="100"/>
-      <c r="B94" s="130" t="s">
+      <c r="B94" s="138" t="s">
         <v>14</v>
       </c>
-      <c r="C94" s="131"/>
-      <c r="D94" s="132"/>
+      <c r="C94" s="139"/>
+      <c r="D94" s="140"/>
       <c r="E94" s="40">
         <f>SUM(E86:E93)</f>
         <v>0</v>
@@ -6902,10 +6902,10 @@
     </row>
     <row r="96" spans="1:27" ht="12" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A96" s="100"/>
-      <c r="B96" s="129" t="s">
+      <c r="B96" s="137" t="s">
         <v>53</v>
       </c>
-      <c r="C96" s="129"/>
+      <c r="C96" s="137"/>
       <c r="D96" s="32"/>
       <c r="E96" s="7"/>
       <c r="F96" s="7"/>
@@ -7241,10 +7241,10 @@
     </row>
     <row r="102" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A102" s="100"/>
-      <c r="B102" s="129" t="s">
+      <c r="B102" s="137" t="s">
         <v>54</v>
       </c>
-      <c r="C102" s="129"/>
+      <c r="C102" s="137"/>
       <c r="D102" s="32"/>
       <c r="E102" s="7"/>
       <c r="F102" s="7"/>
@@ -7592,11 +7592,11 @@
     </row>
     <row r="108" spans="1:27" x14ac:dyDescent="0.15">
       <c r="A108" s="100"/>
-      <c r="B108" s="130" t="s">
+      <c r="B108" s="138" t="s">
         <v>15</v>
       </c>
-      <c r="C108" s="131"/>
-      <c r="D108" s="132"/>
+      <c r="C108" s="139"/>
+      <c r="D108" s="140"/>
       <c r="E108" s="40">
         <f>SUM(E97:E107)</f>
         <v>0</v>
@@ -7697,13 +7697,13 @@
     </row>
     <row r="110" spans="1:27" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A110" s="100"/>
-      <c r="B110" s="120" t="s">
+      <c r="B110" s="146" t="s">
         <v>60</v>
       </c>
-      <c r="C110" s="121"/>
+      <c r="C110" s="147"/>
       <c r="D110" s="112">
         <f>F59</f>
-        <v>46142</v>
+        <v>46507</v>
       </c>
       <c r="E110" s="18">
         <f>E64+E75+E83+E94+E108</f>
@@ -7805,6 +7805,44 @@
     </row>
   </sheetData>
   <mergeCells count="54">
+    <mergeCell ref="B110:C110"/>
+    <mergeCell ref="M1:M4"/>
+    <mergeCell ref="H1:H4"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:G3"/>
+    <mergeCell ref="J2:J3"/>
+    <mergeCell ref="K2:K3"/>
+    <mergeCell ref="B102:C102"/>
+    <mergeCell ref="B94:D94"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="B55:D55"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B64:D64"/>
+    <mergeCell ref="B85:C85"/>
+    <mergeCell ref="B83:D83"/>
+    <mergeCell ref="B49:C49"/>
+    <mergeCell ref="A1:A4"/>
+    <mergeCell ref="B108:D108"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="I2:I4"/>
+    <mergeCell ref="B13:C13"/>
+    <mergeCell ref="B77:C77"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B1:B4"/>
+    <mergeCell ref="B6:C6"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="B57:C57"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B66:C66"/>
+    <mergeCell ref="B75:D75"/>
+    <mergeCell ref="W2:W4"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B30:D30"/>
     <mergeCell ref="Z2:Z4"/>
     <mergeCell ref="U1:U4"/>
     <mergeCell ref="C2:C4"/>
@@ -7821,44 +7859,6 @@
     <mergeCell ref="T1:T4"/>
     <mergeCell ref="X2:X4"/>
     <mergeCell ref="V2:V4"/>
-    <mergeCell ref="W2:W4"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="A1:A4"/>
-    <mergeCell ref="B108:D108"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="I2:I4"/>
-    <mergeCell ref="B13:C13"/>
-    <mergeCell ref="B77:C77"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B1:B4"/>
-    <mergeCell ref="B6:C6"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="B57:C57"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B66:C66"/>
-    <mergeCell ref="B75:D75"/>
-    <mergeCell ref="B110:C110"/>
-    <mergeCell ref="M1:M4"/>
-    <mergeCell ref="H1:H4"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:G3"/>
-    <mergeCell ref="J2:J3"/>
-    <mergeCell ref="K2:K3"/>
-    <mergeCell ref="B102:C102"/>
-    <mergeCell ref="B94:D94"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="B55:D55"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B64:D64"/>
-    <mergeCell ref="B85:C85"/>
-    <mergeCell ref="B83:D83"/>
-    <mergeCell ref="B49:C49"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>
@@ -7906,20 +7906,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" s="5" customFormat="1" ht="9" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A1" s="166"/>
-      <c r="B1" s="167"/>
-      <c r="C1" s="167"/>
-      <c r="D1" s="167"/>
-      <c r="E1" s="167"/>
-      <c r="F1" s="167"/>
-      <c r="G1" s="167"/>
-      <c r="H1" s="167"/>
-      <c r="I1" s="167"/>
-      <c r="J1" s="167"/>
-      <c r="K1" s="167"/>
-      <c r="L1" s="167"/>
-      <c r="M1" s="167"/>
-      <c r="N1" s="167"/>
+      <c r="A1" s="157"/>
+      <c r="B1" s="158"/>
+      <c r="C1" s="158"/>
+      <c r="D1" s="158"/>
+      <c r="E1" s="158"/>
+      <c r="F1" s="158"/>
+      <c r="G1" s="158"/>
+      <c r="H1" s="158"/>
+      <c r="I1" s="158"/>
+      <c r="J1" s="158"/>
+      <c r="K1" s="158"/>
+      <c r="L1" s="158"/>
+      <c r="M1" s="158"/>
+      <c r="N1" s="158"/>
       <c r="O1" s="70"/>
       <c r="P1" s="2"/>
       <c r="Q1" s="2"/>
@@ -7936,12 +7936,12 @@
       <c r="B2" s="46"/>
       <c r="C2" s="47"/>
       <c r="D2" s="48"/>
-      <c r="E2" s="174" t="s">
+      <c r="E2" s="167" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="175"/>
-      <c r="G2" s="176"/>
-      <c r="H2" s="177"/>
+      <c r="F2" s="168"/>
+      <c r="G2" s="169"/>
+      <c r="H2" s="170"/>
       <c r="I2" s="49"/>
       <c r="J2" s="49"/>
       <c r="K2" s="49"/>
@@ -7996,20 +7996,20 @@
         <v>3</v>
       </c>
       <c r="F4" s="49"/>
-      <c r="G4" s="163" t="s">
+      <c r="G4" s="177" t="s">
         <v>52</v>
       </c>
-      <c r="H4" s="164"/>
-      <c r="I4" s="165"/>
+      <c r="H4" s="178"/>
+      <c r="I4" s="179"/>
       <c r="J4" s="49"/>
       <c r="K4" s="106" t="s">
         <v>26</v>
       </c>
       <c r="L4" s="49"/>
-      <c r="M4" s="160" t="s">
+      <c r="M4" s="174" t="s">
         <v>65</v>
       </c>
-      <c r="N4" s="161"/>
+      <c r="N4" s="175"/>
       <c r="O4" s="71"/>
       <c r="P4" s="2"/>
       <c r="Q4" s="2"/>
@@ -8038,8 +8038,8 @@
       <c r="J5" s="49"/>
       <c r="K5" s="49"/>
       <c r="L5" s="49"/>
-      <c r="M5" s="161"/>
-      <c r="N5" s="161"/>
+      <c r="M5" s="175"/>
+      <c r="N5" s="175"/>
       <c r="O5" s="71"/>
       <c r="P5" s="2"/>
       <c r="Q5" s="2"/>
@@ -8053,29 +8053,29 @@
     </row>
     <row r="6" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="63"/>
-      <c r="B6" s="157" t="s">
+      <c r="B6" s="159" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="158"/>
-      <c r="D6" s="159"/>
+      <c r="C6" s="160"/>
+      <c r="D6" s="173"/>
       <c r="E6" s="52">
         <f>Schedule!E64</f>
         <v>0</v>
       </c>
       <c r="F6" s="49"/>
-      <c r="G6" s="157" t="s">
+      <c r="G6" s="159" t="s">
         <v>21</v>
       </c>
-      <c r="H6" s="158"/>
-      <c r="I6" s="158"/>
-      <c r="J6" s="168"/>
+      <c r="H6" s="160"/>
+      <c r="I6" s="160"/>
+      <c r="J6" s="161"/>
       <c r="K6" s="52">
         <f>Schedule!V11+Schedule!V64</f>
         <v>0</v>
       </c>
       <c r="L6" s="49"/>
-      <c r="M6" s="161"/>
-      <c r="N6" s="161"/>
+      <c r="M6" s="175"/>
+      <c r="N6" s="175"/>
       <c r="O6" s="71"/>
       <c r="P6" s="2"/>
       <c r="Q6" s="2"/>
@@ -8089,29 +8089,29 @@
     </row>
     <row r="7" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="63"/>
-      <c r="B7" s="157" t="s">
+      <c r="B7" s="159" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="158"/>
-      <c r="D7" s="159"/>
+      <c r="C7" s="160"/>
+      <c r="D7" s="173"/>
       <c r="E7" s="52">
         <f>Schedule!E75</f>
         <v>0</v>
       </c>
       <c r="F7" s="49"/>
-      <c r="G7" s="157" t="s">
+      <c r="G7" s="159" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="158"/>
-      <c r="I7" s="158"/>
-      <c r="J7" s="168"/>
+      <c r="H7" s="160"/>
+      <c r="I7" s="160"/>
+      <c r="J7" s="161"/>
       <c r="K7" s="52">
         <f>Schedule!V22+Schedule!V75</f>
         <v>0</v>
       </c>
       <c r="L7" s="49"/>
-      <c r="M7" s="161"/>
-      <c r="N7" s="161"/>
+      <c r="M7" s="175"/>
+      <c r="N7" s="175"/>
       <c r="O7" s="71"/>
       <c r="P7" s="2"/>
       <c r="Q7" s="2"/>
@@ -8125,29 +8125,29 @@
     </row>
     <row r="8" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A8" s="63"/>
-      <c r="B8" s="157" t="s">
+      <c r="B8" s="159" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="158"/>
-      <c r="D8" s="159"/>
+      <c r="C8" s="160"/>
+      <c r="D8" s="173"/>
       <c r="E8" s="52">
         <f>Schedule!E83</f>
         <v>0</v>
       </c>
       <c r="F8" s="49"/>
-      <c r="G8" s="157" t="s">
+      <c r="G8" s="159" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="158"/>
-      <c r="I8" s="158"/>
-      <c r="J8" s="168"/>
+      <c r="H8" s="160"/>
+      <c r="I8" s="160"/>
+      <c r="J8" s="161"/>
       <c r="K8" s="52">
         <f>Schedule!V30+Schedule!V83</f>
         <v>0</v>
       </c>
       <c r="L8" s="49"/>
-      <c r="M8" s="161"/>
-      <c r="N8" s="161"/>
+      <c r="M8" s="175"/>
+      <c r="N8" s="175"/>
       <c r="O8" s="71"/>
       <c r="P8" s="2"/>
       <c r="Q8" s="2"/>
@@ -8161,29 +8161,29 @@
     </row>
     <row r="9" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A9" s="63"/>
-      <c r="B9" s="157" t="s">
+      <c r="B9" s="159" t="s">
         <v>14</v>
       </c>
-      <c r="C9" s="158"/>
-      <c r="D9" s="159"/>
+      <c r="C9" s="160"/>
+      <c r="D9" s="173"/>
       <c r="E9" s="52">
         <f>Schedule!E94</f>
         <v>0</v>
       </c>
       <c r="F9" s="49"/>
-      <c r="G9" s="157" t="s">
+      <c r="G9" s="159" t="s">
         <v>24</v>
       </c>
-      <c r="H9" s="158"/>
-      <c r="I9" s="158"/>
-      <c r="J9" s="168"/>
+      <c r="H9" s="160"/>
+      <c r="I9" s="160"/>
+      <c r="J9" s="161"/>
       <c r="K9" s="52">
         <f>Schedule!V41+Schedule!V94</f>
         <v>0</v>
       </c>
       <c r="L9" s="49"/>
-      <c r="M9" s="161"/>
-      <c r="N9" s="161"/>
+      <c r="M9" s="175"/>
+      <c r="N9" s="175"/>
       <c r="O9" s="71"/>
       <c r="P9" s="2"/>
       <c r="Q9" s="2"/>
@@ -8197,29 +8197,29 @@
     </row>
     <row r="10" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A10" s="63"/>
-      <c r="B10" s="157" t="s">
+      <c r="B10" s="159" t="s">
         <v>15</v>
       </c>
-      <c r="C10" s="158"/>
-      <c r="D10" s="159"/>
+      <c r="C10" s="160"/>
+      <c r="D10" s="173"/>
       <c r="E10" s="52">
         <f>Schedule!E108</f>
         <v>0</v>
       </c>
       <c r="F10" s="49"/>
-      <c r="G10" s="157" t="s">
+      <c r="G10" s="159" t="s">
         <v>25</v>
       </c>
-      <c r="H10" s="158"/>
-      <c r="I10" s="158"/>
-      <c r="J10" s="168"/>
+      <c r="H10" s="160"/>
+      <c r="I10" s="160"/>
+      <c r="J10" s="161"/>
       <c r="K10" s="52">
         <f>Schedule!V55+Schedule!V108</f>
         <v>0</v>
       </c>
       <c r="L10" s="49"/>
-      <c r="M10" s="161"/>
-      <c r="N10" s="161"/>
+      <c r="M10" s="175"/>
+      <c r="N10" s="175"/>
       <c r="O10" s="71"/>
       <c r="P10" s="2"/>
       <c r="Q10" s="2"/>
@@ -8233,29 +8233,29 @@
     </row>
     <row r="11" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A11" s="63"/>
-      <c r="B11" s="178" t="s">
+      <c r="B11" s="171" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="178"/>
-      <c r="D11" s="179"/>
+      <c r="C11" s="171"/>
+      <c r="D11" s="172"/>
       <c r="E11" s="53">
         <f>SUM(E6:E10)</f>
         <v>0</v>
       </c>
       <c r="F11" s="49"/>
-      <c r="G11" s="172" t="s">
+      <c r="G11" s="165" t="s">
         <v>19</v>
       </c>
-      <c r="H11" s="172"/>
-      <c r="I11" s="172"/>
-      <c r="J11" s="173"/>
+      <c r="H11" s="165"/>
+      <c r="I11" s="165"/>
+      <c r="J11" s="166"/>
       <c r="K11" s="53">
         <f>SUM(K6:K10)</f>
         <v>0</v>
       </c>
       <c r="L11" s="49"/>
-      <c r="M11" s="161"/>
-      <c r="N11" s="161"/>
+      <c r="M11" s="175"/>
+      <c r="N11" s="175"/>
       <c r="O11" s="71"/>
       <c r="P11" s="2"/>
       <c r="Q11" s="2"/>
@@ -8280,8 +8280,8 @@
       <c r="J12" s="49"/>
       <c r="K12" s="49"/>
       <c r="L12" s="49"/>
-      <c r="M12" s="161"/>
-      <c r="N12" s="161"/>
+      <c r="M12" s="175"/>
+      <c r="N12" s="175"/>
       <c r="O12" s="71"/>
       <c r="P12" s="2"/>
       <c r="Q12" s="2"/>
@@ -8295,29 +8295,29 @@
     </row>
     <row r="13" spans="1:24" s="5" customFormat="1" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A13" s="63"/>
-      <c r="B13" s="178" t="s">
+      <c r="B13" s="171" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="178"/>
-      <c r="D13" s="179"/>
+      <c r="C13" s="171"/>
+      <c r="D13" s="172"/>
       <c r="E13" s="53" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="F13" s="49"/>
-      <c r="G13" s="172" t="s">
+      <c r="G13" s="165" t="s">
         <v>27</v>
       </c>
-      <c r="H13" s="172"/>
-      <c r="I13" s="172"/>
-      <c r="J13" s="173"/>
+      <c r="H13" s="165"/>
+      <c r="I13" s="165"/>
+      <c r="J13" s="166"/>
       <c r="K13" s="53" t="e">
         <f>#REF!</f>
         <v>#REF!</v>
       </c>
       <c r="L13" s="49"/>
-      <c r="M13" s="162"/>
-      <c r="N13" s="162"/>
+      <c r="M13" s="176"/>
+      <c r="N13" s="176"/>
       <c r="O13" s="71"/>
       <c r="P13" s="2"/>
       <c r="Q13" s="2"/>
@@ -8342,8 +8342,8 @@
       <c r="J14" s="49"/>
       <c r="K14" s="49"/>
       <c r="L14" s="49"/>
-      <c r="M14" s="162"/>
-      <c r="N14" s="162"/>
+      <c r="M14" s="176"/>
+      <c r="N14" s="176"/>
       <c r="O14" s="71"/>
       <c r="P14" s="2"/>
       <c r="Q14" s="2"/>
@@ -8357,31 +8357,31 @@
     </row>
     <row r="15" spans="1:24" s="5" customFormat="1" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.2">
       <c r="A15" s="63"/>
-      <c r="B15" s="169" t="e">
+      <c r="B15" s="162" t="e">
         <f>IF(E15&gt;0,"Purchases exceed Assets listed on Schedule",IF(E15&lt;0,"Assets listed on Schedule exceed Purchase values","Purchases reconcile with Fixed asset Schedule"))</f>
         <v>#REF!</v>
       </c>
-      <c r="C15" s="170"/>
-      <c r="D15" s="171"/>
+      <c r="C15" s="163"/>
+      <c r="D15" s="164"/>
       <c r="E15" s="104" t="e">
         <f>E13-E11</f>
         <v>#REF!</v>
       </c>
       <c r="F15" s="49"/>
-      <c r="G15" s="169" t="e">
+      <c r="G15" s="162" t="e">
         <f>IF(K15&gt;0,"Sales exceed Assets listed on Schedule",IF(K15&lt;0,"Assets listed on Schedule exceed Sales values","Sales reconcile with Fixed asset Schedule"))</f>
         <v>#REF!</v>
       </c>
-      <c r="H15" s="170"/>
-      <c r="I15" s="170"/>
-      <c r="J15" s="171"/>
+      <c r="H15" s="163"/>
+      <c r="I15" s="163"/>
+      <c r="J15" s="164"/>
       <c r="K15" s="104" t="e">
         <f>K13-K11</f>
         <v>#REF!</v>
       </c>
       <c r="L15" s="49"/>
-      <c r="M15" s="162"/>
-      <c r="N15" s="162"/>
+      <c r="M15" s="176"/>
+      <c r="N15" s="176"/>
       <c r="O15" s="71"/>
       <c r="P15" s="2"/>
       <c r="Q15" s="2"/>
@@ -8421,6 +8421,10 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="M4:N15"/>
+    <mergeCell ref="G4:I4"/>
     <mergeCell ref="A1:N1"/>
     <mergeCell ref="G6:J6"/>
     <mergeCell ref="G15:J15"/>
@@ -8437,10 +8441,6 @@
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B6:D6"/>
     <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="M4:N15"/>
-    <mergeCell ref="G4:I4"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -8495,22 +8495,22 @@
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="90"/>
       <c r="B2" s="80"/>
-      <c r="C2" s="184" t="s">
+      <c r="C2" s="185" t="s">
         <v>47</v>
       </c>
-      <c r="D2" s="185"/>
+      <c r="D2" s="186"/>
       <c r="E2" s="83">
         <f>SUM(E8:E26)</f>
         <v>0</v>
       </c>
       <c r="F2" s="81"/>
-      <c r="G2" s="180" t="s">
+      <c r="G2" s="183" t="s">
         <v>48</v>
       </c>
-      <c r="H2" s="181"/>
-      <c r="I2" s="181"/>
-      <c r="J2" s="181"/>
-      <c r="K2" s="181"/>
+      <c r="H2" s="184"/>
+      <c r="I2" s="184"/>
+      <c r="J2" s="184"/>
+      <c r="K2" s="184"/>
       <c r="L2" s="87"/>
       <c r="M2" s="90"/>
     </row>
@@ -8523,11 +8523,11 @@
       <c r="D3" s="95"/>
       <c r="E3" s="81"/>
       <c r="F3" s="81"/>
-      <c r="G3" s="181"/>
-      <c r="H3" s="181"/>
-      <c r="I3" s="181"/>
-      <c r="J3" s="181"/>
-      <c r="K3" s="181"/>
+      <c r="G3" s="184"/>
+      <c r="H3" s="184"/>
+      <c r="I3" s="184"/>
+      <c r="J3" s="184"/>
+      <c r="K3" s="184"/>
       <c r="L3" s="87"/>
       <c r="M3" s="90"/>
     </row>
@@ -8548,46 +8548,46 @@
     </row>
     <row r="5" spans="1:13" s="85" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="93"/>
-      <c r="B5" s="138" t="s">
+      <c r="B5" s="122" t="s">
         <v>38</v>
       </c>
-      <c r="C5" s="148" t="s">
+      <c r="C5" s="125" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="148" t="s">
+      <c r="D5" s="125" t="s">
         <v>66</v>
       </c>
-      <c r="E5" s="182" t="s">
+      <c r="E5" s="181" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="182" t="s">
+      <c r="F5" s="181" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="182" t="s">
+      <c r="G5" s="181" t="s">
         <v>37</v>
       </c>
-      <c r="H5" s="148" t="s">
+      <c r="H5" s="125" t="s">
         <v>35</v>
       </c>
-      <c r="I5" s="182" t="s">
+      <c r="I5" s="181" t="s">
         <v>46</v>
       </c>
-      <c r="J5" s="183"/>
-      <c r="K5" s="183"/>
-      <c r="L5" s="148" t="s">
+      <c r="J5" s="182"/>
+      <c r="K5" s="182"/>
+      <c r="L5" s="125" t="s">
         <v>45</v>
       </c>
       <c r="M5" s="93"/>
     </row>
     <row r="6" spans="1:13" s="85" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="93"/>
-      <c r="B6" s="186"/>
-      <c r="C6" s="186"/>
-      <c r="D6" s="186"/>
-      <c r="E6" s="186"/>
-      <c r="F6" s="186"/>
-      <c r="G6" s="186"/>
-      <c r="H6" s="186"/>
+      <c r="B6" s="180"/>
+      <c r="C6" s="180"/>
+      <c r="D6" s="180"/>
+      <c r="E6" s="180"/>
+      <c r="F6" s="180"/>
+      <c r="G6" s="180"/>
+      <c r="H6" s="180"/>
       <c r="I6" s="84" t="s">
         <v>34</v>
       </c>
@@ -8597,7 +8597,7 @@
       <c r="K6" s="84" t="s">
         <v>36</v>
       </c>
-      <c r="L6" s="186"/>
+      <c r="L6" s="180"/>
       <c r="M6" s="93"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.15">
@@ -9056,46 +9056,46 @@
     </row>
     <row r="31" spans="1:13" s="85" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A31" s="93"/>
-      <c r="B31" s="138" t="s">
+      <c r="B31" s="122" t="s">
         <v>38</v>
       </c>
-      <c r="C31" s="148" t="s">
+      <c r="C31" s="125" t="s">
         <v>33</v>
       </c>
-      <c r="D31" s="148" t="s">
+      <c r="D31" s="125" t="s">
         <v>66</v>
       </c>
-      <c r="E31" s="182" t="s">
+      <c r="E31" s="181" t="s">
         <v>44</v>
       </c>
-      <c r="F31" s="182" t="s">
+      <c r="F31" s="181" t="s">
         <v>43</v>
       </c>
-      <c r="G31" s="182" t="s">
+      <c r="G31" s="181" t="s">
         <v>37</v>
       </c>
-      <c r="H31" s="148" t="s">
+      <c r="H31" s="125" t="s">
         <v>35</v>
       </c>
-      <c r="I31" s="182" t="s">
+      <c r="I31" s="181" t="s">
         <v>46</v>
       </c>
-      <c r="J31" s="183"/>
-      <c r="K31" s="183"/>
-      <c r="L31" s="148" t="s">
+      <c r="J31" s="182"/>
+      <c r="K31" s="182"/>
+      <c r="L31" s="125" t="s">
         <v>45</v>
       </c>
       <c r="M31" s="93"/>
     </row>
     <row r="32" spans="1:13" s="85" customFormat="1" ht="30.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A32" s="93"/>
-      <c r="B32" s="186"/>
-      <c r="C32" s="186"/>
-      <c r="D32" s="186"/>
-      <c r="E32" s="186"/>
-      <c r="F32" s="186"/>
-      <c r="G32" s="186"/>
-      <c r="H32" s="186"/>
+      <c r="B32" s="180"/>
+      <c r="C32" s="180"/>
+      <c r="D32" s="180"/>
+      <c r="E32" s="180"/>
+      <c r="F32" s="180"/>
+      <c r="G32" s="180"/>
+      <c r="H32" s="180"/>
       <c r="I32" s="84" t="s">
         <v>34</v>
       </c>
@@ -9105,7 +9105,7 @@
       <c r="K32" s="84" t="s">
         <v>36</v>
       </c>
-      <c r="L32" s="186"/>
+      <c r="L32" s="180"/>
       <c r="M32" s="93"/>
     </row>
     <row r="33" spans="1:13" s="85" customFormat="1" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -9530,6 +9530,16 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="G2:K3"/>
+    <mergeCell ref="I31:K31"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="G5:G6"/>
+    <mergeCell ref="H5:H6"/>
     <mergeCell ref="L31:L32"/>
     <mergeCell ref="L5:L6"/>
     <mergeCell ref="I5:K5"/>
@@ -9540,16 +9550,6 @@
     <mergeCell ref="F31:F32"/>
     <mergeCell ref="G31:G32"/>
     <mergeCell ref="H31:H32"/>
-    <mergeCell ref="G2:K3"/>
-    <mergeCell ref="I31:K31"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
-    <mergeCell ref="D5:D6"/>
-    <mergeCell ref="E5:E6"/>
-    <mergeCell ref="F5:F6"/>
-    <mergeCell ref="G5:G6"/>
-    <mergeCell ref="H5:H6"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <printOptions horizontalCentered="1" verticalCentered="1"/>

</xml_diff>